<commit_message>
Updating results for ACC vs F1 with RFE
</commit_message>
<xml_diff>
--- a/RFE/results.xlsx
+++ b/RFE/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="95">
   <si>
     <t>Accuracy</t>
   </si>
@@ -105,9 +105,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>F1 'inversa'</t>
-  </si>
-  <si>
     <t>0.001</t>
   </si>
   <si>
@@ -138,6 +135,201 @@
   </si>
   <si>
     <t>Nota</t>
+  </si>
+  <si>
+    <t>Nº características</t>
+  </si>
+  <si>
+    <t>F1 inversa'</t>
+  </si>
+  <si>
+    <t>0.8391539055952808</t>
+  </si>
+  <si>
+    <t>0.8634280573060081</t>
+  </si>
+  <si>
+    <t>24 29
+27 330</t>
+  </si>
+  <si>
+    <t>0.400859341174323</t>
+  </si>
+  <si>
+    <t>0.516851775675305</t>
+  </si>
+  <si>
+    <t>33 20
+47 310</t>
+  </si>
+  <si>
+    <t>0.8196990309929874</t>
+  </si>
+  <si>
+    <t>0.9048965509735419</t>
+  </si>
+  <si>
+    <t>2 35
+4 369</t>
+  </si>
+  <si>
+    <t>0.22122871280766016</t>
+  </si>
+  <si>
+    <t>0.5309523809523808</t>
+  </si>
+  <si>
+    <t>29 8
+44 329</t>
+  </si>
+  <si>
+    <t>0.8537013455810596</t>
+  </si>
+  <si>
+    <t>0.9245306428967904</t>
+  </si>
+  <si>
+    <t>8 20
+11 371</t>
+  </si>
+  <si>
+    <t>14 14
+37 345</t>
+  </si>
+  <si>
+    <t>0.13704942400594575</t>
+  </si>
+  <si>
+    <t>0.3516488413547237</t>
+  </si>
+  <si>
+    <t>0.0001</t>
+  </si>
+  <si>
+    <t>0.9121283689409851</t>
+  </si>
+  <si>
+    <t>0.9439884198038767</t>
+  </si>
+  <si>
+    <t>3 23
+0 384</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>0.2220779220779221</t>
+  </si>
+  <si>
+    <t>0.5569230769230769</t>
+  </si>
+  <si>
+    <t>16 10
+14 370</t>
+  </si>
+  <si>
+    <t>0.8878048780487804</t>
+  </si>
+  <si>
+    <t>0.8878048780487806</t>
+  </si>
+  <si>
+    <t>12 13
+33 352</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.20555555555555555</t>
+  </si>
+  <si>
+    <t>0.44940836940836953</t>
+  </si>
+  <si>
+    <t>10 15
+9 376</t>
+  </si>
+  <si>
+    <t>0.9414568844483625</t>
+  </si>
+  <si>
+    <t>0.9561218677782494</t>
+  </si>
+  <si>
+    <t>2 16
+2 390</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>0.2961038961038961</t>
+  </si>
+  <si>
+    <t>0.515032679738562</t>
+  </si>
+  <si>
+    <t>13 5
+22 370</t>
+  </si>
+  <si>
+    <t>0.9390773573063708</t>
+  </si>
+  <si>
+    <t>0.9732266010745784</t>
+  </si>
+  <si>
+    <t>1 11
+0 398</t>
+  </si>
+  <si>
+    <t>0.16</t>
+  </si>
+  <si>
+    <t>0.2942857142857143</t>
+  </si>
+  <si>
+    <t>4 8
+12 386</t>
+  </si>
+  <si>
+    <t>0.9365853658536585</t>
+  </si>
+  <si>
+    <t>0.975609756097561</t>
+  </si>
+  <si>
+    <t>0 10
+0 400</t>
+  </si>
+  <si>
+    <t>6 4
+11 389</t>
+  </si>
+  <si>
+    <t>0.08888888888888889</t>
+  </si>
+  <si>
+    <t>0.40428571428571436</t>
+  </si>
+  <si>
+    <t>0.9610300279709625</t>
+  </si>
+  <si>
+    <t>0.9757258482892727</t>
+  </si>
+  <si>
+    <t>1 7
+3 399</t>
+  </si>
+  <si>
+    <t>0.15506787330316746</t>
+  </si>
+  <si>
+    <t>6 2
+69 333</t>
   </si>
 </sst>
 </file>
@@ -185,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -287,11 +479,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -299,7 +502,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -311,12 +513,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,65 +851,77 @@
     <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="7" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1"/>
-    <col min="9" max="10" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="G1" s="9" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="19"/>
+      <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="L2" s="20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M2" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -712,228 +931,452 @@
       <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="9">
+        <v>27</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="22"/>
-    </row>
-    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M3" s="22">
+        <v>27</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2">
+        <v>7</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="K4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="18"/>
-      <c r="G5" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2">
         <v>5</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G5" s="25"/>
+      <c r="H5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="18"/>
-      <c r="G6" s="2" t="s">
+      <c r="B6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2">
+        <v>9</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="18"/>
-      <c r="G7" s="2" t="s">
+      <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="25"/>
+      <c r="H7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="18"/>
-      <c r="G8" s="2" t="s">
+      <c r="B8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="2">
+        <v>70</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="18"/>
-      <c r="G9" s="2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="2">
+        <v>48</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="18"/>
-      <c r="G10" s="2" t="s">
+      <c r="B10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="2">
+        <v>67</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="18"/>
-      <c r="G11" s="2" t="s">
+      <c r="B11" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="18"/>
-      <c r="G12" s="2" t="s">
+      <c r="B12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="25"/>
+      <c r="H12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="18"/>
-      <c r="G13" s="2" t="s">
+      <c r="B13" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="2">
+        <v>89</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="19"/>
-      <c r="G14" s="3" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
+      <c r="I14" s="10"/>
       <c r="J14" s="11"/>
-      <c r="K14" s="20"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K14" s="10"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="11"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
@@ -941,7 +1384,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="D16" s="1"/>
@@ -975,7 +1418,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1"/>
       <c r="D20" s="1"/>

</xml_diff>

<commit_message>
Updating results for RFE
</commit_message>
<xml_diff>
--- a/RFE/results.xlsx
+++ b/RFE/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="95">
   <si>
     <t>Accuracy</t>
   </si>
@@ -377,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -490,11 +490,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -524,6 +533,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,7 +851,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -920,6 +930,9 @@
       <c r="M2" s="20" t="s">
         <v>36</v>
       </c>
+      <c r="N2" s="27" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">

</xml_diff>